<commit_message>
Fixed bug where "Remaining ___ Upgrades" calculations did not account for 'skips'
</commit_message>
<xml_diff>
--- a/ClashOfClans-Calculator.xlsx
+++ b/ClashOfClans-Calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <workbookProtection workbookPassword="9AF0" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="669" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="669"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="264">
   <si>
     <t>Time</t>
   </si>
@@ -874,6 +874,9 @@
 2. Enter quantities for an "Attack Set" and give it a name in the header
 3. Type the name of the "Attack Set" in the small red box
 4. View the calculated values in the tables</t>
+  </si>
+  <si>
+    <t>Fixed bug where "Remaining ___ Upgrades" calculations did not account for 'skips'</t>
   </si>
 </sst>
 </file>
@@ -2224,7 +2227,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1188">
+  <cellStyleXfs count="1190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3012,6 +3015,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4024,6 +4029,18 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="59" xfId="786" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4152,20 +4169,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="59" xfId="786" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1188">
+  <cellStyles count="1190">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5000,6 +5005,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1185" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1189" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5355,7 +5362,29 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Upgrade Costs" xfId="447"/>
   </cellStyles>
-  <dxfs count="271">
+  <dxfs count="273">
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="#\ ??/24"/>
     </dxf>
@@ -7982,120 +8011,120 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
     <tableStyle name="Custom" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="270"/>
-      <tableStyleElement type="headerRow" dxfId="269"/>
-      <tableStyleElement type="totalRow" dxfId="268"/>
-      <tableStyleElement type="firstColumn" dxfId="267"/>
-      <tableStyleElement type="lastColumn" dxfId="266"/>
-      <tableStyleElement type="firstRowStripe" dxfId="265"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="264"/>
+      <tableStyleElement type="wholeTable" dxfId="272"/>
+      <tableStyleElement type="headerRow" dxfId="271"/>
+      <tableStyleElement type="totalRow" dxfId="270"/>
+      <tableStyleElement type="firstColumn" dxfId="269"/>
+      <tableStyleElement type="lastColumn" dxfId="268"/>
+      <tableStyleElement type="firstRowStripe" dxfId="267"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="266"/>
     </tableStyle>
     <tableStyle name="TableStyleMedium14 2" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="263"/>
-      <tableStyleElement type="headerRow" dxfId="262"/>
-      <tableStyleElement type="totalRow" dxfId="261"/>
-      <tableStyleElement type="firstColumn" dxfId="260"/>
-      <tableStyleElement type="lastColumn" dxfId="259"/>
-      <tableStyleElement type="firstRowStripe" dxfId="258"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="257"/>
+      <tableStyleElement type="wholeTable" dxfId="265"/>
+      <tableStyleElement type="headerRow" dxfId="264"/>
+      <tableStyleElement type="totalRow" dxfId="263"/>
+      <tableStyleElement type="firstColumn" dxfId="262"/>
+      <tableStyleElement type="lastColumn" dxfId="261"/>
+      <tableStyleElement type="firstRowStripe" dxfId="260"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="259"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ConstructionState" displayName="ConstructionState" ref="A23:S72" totalsRowShown="0" headerRowDxfId="249" dataDxfId="248">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ConstructionState" displayName="ConstructionState" ref="A23:S72" totalsRowShown="0" headerRowDxfId="251" dataDxfId="250">
   <tableColumns count="19">
-    <tableColumn id="1" name="Building or Upgrade" dataDxfId="247"/>
-    <tableColumn id="14" name="Kind" dataDxfId="246">
+    <tableColumn id="1" name="Building or Upgrade" dataDxfId="249"/>
+    <tableColumn id="14" name="Kind" dataDxfId="248">
       <calculatedColumnFormula>VLOOKUP(ConstructionState[[#This Row],[Building or Upgrade]],Upgrades[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Resource" dataDxfId="245">
+    <tableColumn id="15" name="Resource" dataDxfId="247">
       <calculatedColumnFormula>VLOOKUP(ConstructionState[Building or Upgrade],Upgrades[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="MatchStr" dataDxfId="244">
+    <tableColumn id="21" name="MatchStr" dataDxfId="246">
       <calculatedColumnFormula>IF(COUNTIF(Skips,ConstructionState[[#This Row],[Building or Upgrade]]),"IGNORE",ConstructionState[Kind]&amp;"-"&amp;ConstructionState[Resource])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Available" dataDxfId="243">
+    <tableColumn id="2" name="Available" dataDxfId="245">
       <calculatedColumnFormula>IF(AND(ConstructionState[[#This Row],[Kind]]="Upgrade",LabLevel=0),0,VLOOKUP(ConstructionState[Building or Upgrade],QuantAvail[],1+IF(ConstructionState[[#This Row],[Kind]]="Upgrade",LabLevel,THLevel),FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Maximum Level" dataDxfId="242">
+    <tableColumn id="3" name="Maximum Level" dataDxfId="244">
       <calculatedColumnFormula>IF(AND(ConstructionState[[#This Row],[Kind]]="Upgrade",LabLevel=0),0,VLOOKUP(ConstructionState[Building or Upgrade],MaxLevel[],1+IF(ConstructionState[[#This Row],[Kind]]="Upgrade",LabLevel,THLevel),FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Not Built/Upgraded" dataDxfId="241">
+    <tableColumn id="4" name="Not Built/Upgraded" dataDxfId="243">
       <calculatedColumnFormula>ConstructionState[[#This Row],[Available]]-SUM(ConstructionState[[#This Row],[1]:[12]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="1" dataDxfId="240"/>
-    <tableColumn id="6" name="2" dataDxfId="239"/>
-    <tableColumn id="7" name="3" dataDxfId="238"/>
-    <tableColumn id="8" name="4" dataDxfId="237"/>
-    <tableColumn id="9" name="5" dataDxfId="236"/>
-    <tableColumn id="10" name="6" dataDxfId="235"/>
-    <tableColumn id="11" name="7" dataDxfId="234"/>
-    <tableColumn id="12" name="8" dataDxfId="233"/>
-    <tableColumn id="13" name="9" dataDxfId="232"/>
-    <tableColumn id="16" name="10" dataDxfId="231"/>
-    <tableColumn id="17" name="11" dataDxfId="230"/>
-    <tableColumn id="18" name="12" dataDxfId="229"/>
+    <tableColumn id="5" name="1" dataDxfId="242"/>
+    <tableColumn id="6" name="2" dataDxfId="241"/>
+    <tableColumn id="7" name="3" dataDxfId="240"/>
+    <tableColumn id="8" name="4" dataDxfId="239"/>
+    <tableColumn id="9" name="5" dataDxfId="238"/>
+    <tableColumn id="10" name="6" dataDxfId="237"/>
+    <tableColumn id="11" name="7" dataDxfId="236"/>
+    <tableColumn id="12" name="8" dataDxfId="235"/>
+    <tableColumn id="13" name="9" dataDxfId="234"/>
+    <tableColumn id="16" name="10" dataDxfId="233"/>
+    <tableColumn id="17" name="11" dataDxfId="232"/>
+    <tableColumn id="18" name="12" dataDxfId="231"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="CostRemaining" displayName="CostRemaining" ref="A19:R68" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="CostRemaining" displayName="CostRemaining" ref="A19:R68" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="A19:R68"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Cost" dataDxfId="44"/>
-    <tableColumn id="15" name="Kind" dataDxfId="43">
+    <tableColumn id="1" name="Cost" dataDxfId="46"/>
+    <tableColumn id="15" name="Kind" dataDxfId="45">
       <calculatedColumnFormula>VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="42">
+    <tableColumn id="2" name="Resource" dataDxfId="44">
       <calculatedColumnFormula>VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="MatchStr" dataDxfId="41">
+    <tableColumn id="18" name="MatchStr" dataDxfId="43">
       <calculatedColumnFormula>IF(COUNTIF(Skips,CostRemaining[[#This Row],[Cost]])&gt;0,"IGNORE",CostRemaining[Kind]&amp;"-"&amp;CostRemaining[Resource])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Next" dataDxfId="40">
+    <tableColumn id="14" name="Next" dataDxfId="42">
       <calculatedColumnFormula>IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;MATCH(TRUE,INDEX(CostRemaining[[#This Row],[1]:[12]]&lt;&gt;0,),0),Upgrades[#Headers],0),FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="39">
+    <tableColumn id="3" name="1" dataDxfId="41">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:G24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="2" dataDxfId="38">
+    <tableColumn id="4" name="2" dataDxfId="40">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:H24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="3" dataDxfId="37">
+    <tableColumn id="5" name="3" dataDxfId="39">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:I24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="4" dataDxfId="36">
+    <tableColumn id="6" name="4" dataDxfId="38">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:J24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="5" dataDxfId="35">
+    <tableColumn id="7" name="5" dataDxfId="37">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:K24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="6" dataDxfId="34">
+    <tableColumn id="8" name="6" dataDxfId="36">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:L24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="7" dataDxfId="33">
+    <tableColumn id="9" name="7" dataDxfId="35">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:M24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="8" dataDxfId="32">
+    <tableColumn id="10" name="8" dataDxfId="34">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:N24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="9" dataDxfId="31">
+    <tableColumn id="11" name="9" dataDxfId="33">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:O24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="10" dataDxfId="30">
+    <tableColumn id="12" name="10" dataDxfId="32">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:P24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="11" dataDxfId="29">
+    <tableColumn id="13" name="11" dataDxfId="31">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:Q24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="12" dataDxfId="28">
+    <tableColumn id="16" name="12" dataDxfId="30">
       <calculatedColumnFormula>IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:R24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Sum" dataDxfId="27">
+    <tableColumn id="17" name="Sum" dataDxfId="29">
       <calculatedColumnFormula>IF(CostRemaining[[#This Row],[MatchStr]]="IGNORE",0,SUM(CostRemaining[[#This Row],[1]:[12]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8104,59 +8133,59 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="TimeRemaining" displayName="TimeRemaining" ref="A73:R122" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="TimeRemaining" displayName="TimeRemaining" ref="A73:R122" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A73:R122"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Time" dataDxfId="24"/>
-    <tableColumn id="15" name="Kind" dataDxfId="23">
+    <tableColumn id="1" name="Time" dataDxfId="26"/>
+    <tableColumn id="15" name="Kind" dataDxfId="25">
       <calculatedColumnFormula>VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("Kind",Upgrades[#Headers],0),FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="22">
+    <tableColumn id="2" name="Resource" dataDxfId="24">
       <calculatedColumnFormula>VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("Resource",Upgrades[#Headers],0),FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="MatchStr" dataDxfId="21">
+    <tableColumn id="18" name="MatchStr" dataDxfId="23">
       <calculatedColumnFormula>IF(COUNTIF(Skips,TimeRemaining[[#This Row],[Time]])&gt;0,"IGNORE",TimeRemaining[Kind]&amp;"-"&amp;TimeRemaining[Resource])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Next" dataDxfId="20">
+    <tableColumn id="14" name="Next" dataDxfId="22">
       <calculatedColumnFormula>IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;MATCH(TRUE,INDEX(TimeRemaining[[#This Row],[1]:[12]]&lt;&gt;0,),0),Upgrades[#Headers],0),FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="19">
+    <tableColumn id="3" name="1" dataDxfId="21">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:G24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="2" dataDxfId="18">
+    <tableColumn id="4" name="2" dataDxfId="20">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:H24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="3" dataDxfId="17">
+    <tableColumn id="5" name="3" dataDxfId="19">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:I24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="4" dataDxfId="16">
+    <tableColumn id="6" name="4" dataDxfId="18">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:J24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="5" dataDxfId="15">
+    <tableColumn id="7" name="5" dataDxfId="17">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:K24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="6" dataDxfId="14">
+    <tableColumn id="8" name="6" dataDxfId="16">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:L24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="7" dataDxfId="13">
+    <tableColumn id="9" name="7" dataDxfId="15">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:M24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="8" dataDxfId="12">
+    <tableColumn id="10" name="8" dataDxfId="14">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:N24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="9" dataDxfId="11">
+    <tableColumn id="11" name="9" dataDxfId="13">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:O24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="10" dataDxfId="10">
+    <tableColumn id="12" name="10" dataDxfId="12">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:P24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="11" dataDxfId="9">
+    <tableColumn id="13" name="11" dataDxfId="11">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:Q24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="12" dataDxfId="8">
+    <tableColumn id="16" name="12" dataDxfId="10">
       <calculatedColumnFormula>IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F24,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G24:R24)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Sum" dataDxfId="7">
+    <tableColumn id="17" name="Sum" dataDxfId="9">
       <calculatedColumnFormula>IF(TimeRemaining[[#This Row],[MatchStr]]="IGNORE",0,SUM(TimeRemaining[[#This Row],[1]:[12]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8172,25 +8201,25 @@
     <tableColumn id="2" name="Level">
       <calculatedColumnFormula>AQLevel</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="MaxLevel" dataDxfId="6">
+    <tableColumn id="3" name="MaxLevel" dataDxfId="8">
       <calculatedColumnFormula>VLOOKUP(HeroNextUpgrade[[#This Row],[Hero]],MaxLevel[],MATCH("L"&amp;THLevel,MaxLevel[#Headers],0),FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Upgradeable" dataDxfId="5">
+    <tableColumn id="6" name="Upgradeable" dataDxfId="7">
       <calculatedColumnFormula>AND(HeroNextUpgrade[[#This Row],[Level]]&lt;HeroNextUpgrade[[#This Row],[MaxLevel]],COUNTIF(Skips,HeroNextUpgrade[[#This Row],[Hero]])=0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Next Level" dataDxfId="4">
+    <tableColumn id="9" name="Next Level" dataDxfId="6">
       <calculatedColumnFormula>HeroNextUpgrade[[#This Row],[Level]]+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Next Cost" dataDxfId="3">
+    <tableColumn id="4" name="Next Cost" dataDxfId="5">
       <calculatedColumnFormula>VLOOKUP(HeroNextUpgrade[[#This Row],[Next Level]],HeroUpgrades[],MATCH(HeroNextUpgrade[[#This Row],[Lookup Key]]&amp;"-Cost",HeroUpgrades[#Headers],0),FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Next Time" dataDxfId="2">
+    <tableColumn id="5" name="Next Time" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(HeroNextUpgrade[[#This Row],[Next Level]],HeroUpgrades[],MATCH(HeroNextUpgrade[[#This Row],[Lookup Key]]&amp;"-Time",HeroUpgrades[#Headers],0),FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost to Max" dataDxfId="1">
+    <tableColumn id="12" name="Cost to Max" dataDxfId="3">
       <calculatedColumnFormula>IF(HeroNextUpgrade[[#This Row],[Upgradeable]],SUM(OFFSET(HeroUpgrades[],HeroNextUpgrade[[#This Row],[Level]],MATCH(HeroNextUpgrade[[#This Row],[Lookup Key]]&amp;"-Cost",HeroUpgrades[#Headers],0)-1,HeroNextUpgrade[[#This Row],[MaxLevel]]-HeroNextUpgrade[[#This Row],[Level]],1)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Time to Max" dataDxfId="0">
+    <tableColumn id="13" name="Time to Max" dataDxfId="2">
       <calculatedColumnFormula>IF(HeroNextUpgrade[[#This Row],[Upgradeable]],SUM(OFFSET(HeroUpgrades[],HeroNextUpgrade[[#This Row],[Level]],MATCH(HeroNextUpgrade[[#This Row],[Lookup Key]]&amp;"-Time",HeroUpgrades[#Headers],0)-1,HeroNextUpgrade[[#This Row],[MaxLevel]]-HeroNextUpgrade[[#This Row],[Level]],1)),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8199,37 +8228,37 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ArmyState" displayName="ArmyState" ref="B17:L37" headerRowDxfId="222" dataDxfId="221" totalsRowDxfId="220">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ArmyState" displayName="ArmyState" ref="B17:L37" headerRowDxfId="224" dataDxfId="223" totalsRowDxfId="222">
   <tableColumns count="11">
-    <tableColumn id="1" name="Name" totalsRowLabel="Total" dataDxfId="219" totalsRowDxfId="218"/>
-    <tableColumn id="4" name="Count" dataDxfId="217" totalsRowDxfId="216">
+    <tableColumn id="1" name="Name" totalsRowLabel="Total" dataDxfId="221" totalsRowDxfId="220"/>
+    <tableColumn id="4" name="Count" dataDxfId="219" totalsRowDxfId="218">
       <calculatedColumnFormula>INDEX(AttackSets[],MATCH(ArmyState[[#This Row],[Name]],AttackSets[Unit Set],0),MATCH(AttackSet,AttackSets[#Headers],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Type" dataDxfId="215" totalsRowDxfId="214">
+    <tableColumn id="12" name="Type" dataDxfId="217" totalsRowDxfId="216">
       <calculatedColumnFormula>INDEX(UnitCosts[Type],MATCH(ArmyState[[#This Row],[Name]],UnitCosts[Name],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Level" dataDxfId="213" totalsRowDxfId="212">
+    <tableColumn id="2" name="Level" dataDxfId="215" totalsRowDxfId="214">
       <calculatedColumnFormula>IFERROR(MATCH(1,OFFSET(ConstructionState[],MATCH(ArmyState[[#This Row],[Name]],ConstructionState[Building or Upgrade],0)-1,L1Offset,1,12)),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="211" totalsRowDxfId="210">
+    <tableColumn id="3" name="Resource" dataDxfId="213" totalsRowDxfId="212">
       <calculatedColumnFormula>INDEX(UnitCosts[Resource],MATCH(ArmyState[[#This Row],[Name]],UnitCosts[Name],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Cost" dataDxfId="209" totalsRowDxfId="208">
+    <tableColumn id="9" name="Cost" dataDxfId="211" totalsRowDxfId="210">
       <calculatedColumnFormula>VLOOKUP(ArmyState[[#This Row],[Name]],UnitCosts[],MATCH(TEXT(ArmyState[[#This Row],[Level]],"#"),UnitCosts[#Headers],0),FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Time" dataDxfId="207" totalsRowDxfId="206">
+    <tableColumn id="7" name="Time" dataDxfId="209" totalsRowDxfId="208">
       <calculatedColumnFormula>INDEX(UnitCosts[Train Time],MATCH(ArmyState[[#This Row],[Name]],UnitCosts[Name],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Space" dataDxfId="205" totalsRowDxfId="204">
+    <tableColumn id="8" name="Space" dataDxfId="207" totalsRowDxfId="206">
       <calculatedColumnFormula>INDEX(UnitCosts[Space],MATCH(ArmyState[[#This Row],[Name]],UnitCosts[Name],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Total Cost" dataDxfId="203" totalsRowDxfId="202">
+    <tableColumn id="6" name="Total Cost" dataDxfId="205" totalsRowDxfId="204">
       <calculatedColumnFormula>ArmyState[[#This Row],[Count]]*ArmyState[[#This Row],[Cost]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Total Time" dataDxfId="201" totalsRowDxfId="200">
+    <tableColumn id="10" name="Total Time" dataDxfId="203" totalsRowDxfId="202">
       <calculatedColumnFormula>ArmyState[[#This Row],[Count]]*ArmyState[[#This Row],[Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Total Space" dataDxfId="199" totalsRowDxfId="198">
+    <tableColumn id="11" name="Total Space" dataDxfId="201" totalsRowDxfId="200">
       <calculatedColumnFormula>ArmyState[[#This Row],[Count]]*ArmyState[[#This Row],[Space]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8238,137 +8267,137 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="AttackSets" displayName="AttackSets" ref="N17:X37" headerRowDxfId="197" dataDxfId="196" totalsRowDxfId="195">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="AttackSets" displayName="AttackSets" ref="N17:X37" headerRowDxfId="199" dataDxfId="198" totalsRowDxfId="197">
   <tableColumns count="11">
-    <tableColumn id="1" name="Unit Set" totalsRowLabel="Total" dataDxfId="194" totalsRowDxfId="193"/>
-    <tableColumn id="2" name="LastUsed" dataDxfId="192"/>
-    <tableColumn id="3" name="Farming" dataDxfId="191"/>
-    <tableColumn id="4" name="War" dataDxfId="190"/>
-    <tableColumn id="6" name="G+Healers" dataDxfId="189"/>
-    <tableColumn id="7" name="WarSaver" dataDxfId="188"/>
-    <tableColumn id="8" name="Cheapo" dataDxfId="187"/>
-    <tableColumn id="9" name="RageT1" dataDxfId="186"/>
-    <tableColumn id="10" name="     " dataDxfId="185"/>
-    <tableColumn id="11" name="      " dataDxfId="184"/>
-    <tableColumn id="12" name="       " dataDxfId="183"/>
+    <tableColumn id="1" name="Unit Set" totalsRowLabel="Total" dataDxfId="196" totalsRowDxfId="195"/>
+    <tableColumn id="2" name="LastUsed" dataDxfId="194"/>
+    <tableColumn id="3" name="Farming" dataDxfId="193"/>
+    <tableColumn id="4" name="War" dataDxfId="192"/>
+    <tableColumn id="6" name="G+Healers" dataDxfId="191"/>
+    <tableColumn id="7" name="WarSaver" dataDxfId="190"/>
+    <tableColumn id="8" name="Cheapo" dataDxfId="189"/>
+    <tableColumn id="9" name="RageT1" dataDxfId="188"/>
+    <tableColumn id="10" name="     " dataDxfId="187"/>
+    <tableColumn id="11" name="      " dataDxfId="186"/>
+    <tableColumn id="12" name="       " dataDxfId="185"/>
   </tableColumns>
   <tableStyleInfo name="Custom" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Upgrades" displayName="Upgrades" ref="A2:AA51" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Upgrades" displayName="Upgrades" ref="A2:AA51" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
   <tableColumns count="27">
-    <tableColumn id="1" name="Building" dataDxfId="125"/>
-    <tableColumn id="3" name="Kind" dataDxfId="124"/>
-    <tableColumn id="2" name="Resource" dataDxfId="123"/>
-    <tableColumn id="5" name="C1" dataDxfId="122"/>
-    <tableColumn id="6" name="C2" dataDxfId="121"/>
-    <tableColumn id="7" name="C3" dataDxfId="120"/>
-    <tableColumn id="8" name="C4" dataDxfId="119"/>
-    <tableColumn id="9" name="C5" dataDxfId="118"/>
-    <tableColumn id="10" name="C6" dataDxfId="117"/>
-    <tableColumn id="11" name="C7" dataDxfId="116"/>
-    <tableColumn id="12" name="C8" dataDxfId="115"/>
-    <tableColumn id="13" name="C9" dataDxfId="114"/>
-    <tableColumn id="14" name="C10" dataDxfId="113"/>
-    <tableColumn id="15" name="C11" dataDxfId="112"/>
-    <tableColumn id="16" name="C12" dataDxfId="111"/>
-    <tableColumn id="17" name="T1" dataDxfId="110" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="18" name="T2" dataDxfId="109" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="19" name="T3" dataDxfId="108" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="20" name="T4" dataDxfId="107" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="21" name="T5" dataDxfId="106" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="22" name="T6" dataDxfId="105" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="23" name="T7" dataDxfId="104" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="24" name="T8" dataDxfId="103" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="25" name="T9" dataDxfId="102" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="26" name="T10" dataDxfId="101" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="27" name="T11" dataDxfId="100" dataCellStyle="Normal_Upgrade Costs"/>
-    <tableColumn id="28" name="T12" dataDxfId="99" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="1" name="Building" dataDxfId="127"/>
+    <tableColumn id="3" name="Kind" dataDxfId="126"/>
+    <tableColumn id="2" name="Resource" dataDxfId="125"/>
+    <tableColumn id="5" name="C1" dataDxfId="124"/>
+    <tableColumn id="6" name="C2" dataDxfId="123"/>
+    <tableColumn id="7" name="C3" dataDxfId="122"/>
+    <tableColumn id="8" name="C4" dataDxfId="121"/>
+    <tableColumn id="9" name="C5" dataDxfId="120"/>
+    <tableColumn id="10" name="C6" dataDxfId="119"/>
+    <tableColumn id="11" name="C7" dataDxfId="118"/>
+    <tableColumn id="12" name="C8" dataDxfId="117"/>
+    <tableColumn id="13" name="C9" dataDxfId="116"/>
+    <tableColumn id="14" name="C10" dataDxfId="115"/>
+    <tableColumn id="15" name="C11" dataDxfId="114"/>
+    <tableColumn id="16" name="C12" dataDxfId="113"/>
+    <tableColumn id="17" name="T1" dataDxfId="112" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="18" name="T2" dataDxfId="111" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="19" name="T3" dataDxfId="110" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="20" name="T4" dataDxfId="109" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="21" name="T5" dataDxfId="108" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="22" name="T6" dataDxfId="107" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="23" name="T7" dataDxfId="106" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="24" name="T8" dataDxfId="105" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="25" name="T9" dataDxfId="104" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="26" name="T10" dataDxfId="103" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="27" name="T11" dataDxfId="102" dataCellStyle="Normal_Upgrade Costs"/>
+    <tableColumn id="28" name="T12" dataDxfId="101" dataCellStyle="Normal_Upgrade Costs"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="UnitCosts" displayName="UnitCosts" ref="A111:K131" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="UnitCosts" displayName="UnitCosts" ref="A111:K131" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
   <tableColumns count="11">
-    <tableColumn id="1" name="Name" dataDxfId="96"/>
-    <tableColumn id="2" name="Type" dataDxfId="95"/>
-    <tableColumn id="3" name="Resource" dataDxfId="94"/>
-    <tableColumn id="16" name="Train Time" dataDxfId="93"/>
-    <tableColumn id="15" name="Space" dataDxfId="92"/>
-    <tableColumn id="4" name="1" dataDxfId="91"/>
-    <tableColumn id="5" name="2" dataDxfId="90"/>
-    <tableColumn id="6" name="3" dataDxfId="89"/>
-    <tableColumn id="7" name="4" dataDxfId="88"/>
-    <tableColumn id="8" name="5" dataDxfId="87"/>
-    <tableColumn id="9" name="6" dataDxfId="86"/>
+    <tableColumn id="1" name="Name" dataDxfId="98"/>
+    <tableColumn id="2" name="Type" dataDxfId="97"/>
+    <tableColumn id="3" name="Resource" dataDxfId="96"/>
+    <tableColumn id="16" name="Train Time" dataDxfId="95"/>
+    <tableColumn id="15" name="Space" dataDxfId="94"/>
+    <tableColumn id="4" name="1" dataDxfId="93"/>
+    <tableColumn id="5" name="2" dataDxfId="92"/>
+    <tableColumn id="6" name="3" dataDxfId="91"/>
+    <tableColumn id="7" name="4" dataDxfId="90"/>
+    <tableColumn id="8" name="5" dataDxfId="89"/>
+    <tableColumn id="9" name="6" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="QuantAvail" displayName="QuantAvail" ref="A135:K186" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="QuantAvail" displayName="QuantAvail" ref="A135:K186" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
   <autoFilter ref="A135:K186"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Quantity Available" dataDxfId="83"/>
-    <tableColumn id="2" name="L1" dataDxfId="82"/>
-    <tableColumn id="3" name="L2" dataDxfId="81"/>
-    <tableColumn id="4" name="L3" dataDxfId="80"/>
-    <tableColumn id="5" name="L4" dataDxfId="79"/>
-    <tableColumn id="6" name="L5" dataDxfId="78"/>
-    <tableColumn id="7" name="L6" dataDxfId="77"/>
-    <tableColumn id="8" name="L7" dataDxfId="76"/>
-    <tableColumn id="9" name="L8" dataDxfId="75"/>
-    <tableColumn id="10" name="L9" dataDxfId="74"/>
-    <tableColumn id="11" name="L10" dataDxfId="73"/>
+    <tableColumn id="1" name="Quantity Available" dataDxfId="85"/>
+    <tableColumn id="2" name="L1" dataDxfId="84"/>
+    <tableColumn id="3" name="L2" dataDxfId="83"/>
+    <tableColumn id="4" name="L3" dataDxfId="82"/>
+    <tableColumn id="5" name="L4" dataDxfId="81"/>
+    <tableColumn id="6" name="L5" dataDxfId="80"/>
+    <tableColumn id="7" name="L6" dataDxfId="79"/>
+    <tableColumn id="8" name="L7" dataDxfId="78"/>
+    <tableColumn id="9" name="L8" dataDxfId="77"/>
+    <tableColumn id="10" name="L9" dataDxfId="76"/>
+    <tableColumn id="11" name="L10" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="MaxLevel" displayName="MaxLevel" ref="A189:K240" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="MaxLevel" displayName="MaxLevel" ref="A189:K240" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <autoFilter ref="A189:K240"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Max Level" dataDxfId="70"/>
-    <tableColumn id="2" name="L1" dataDxfId="69"/>
-    <tableColumn id="3" name="L2" dataDxfId="68"/>
-    <tableColumn id="4" name="L3" dataDxfId="67"/>
-    <tableColumn id="5" name="L4" dataDxfId="66"/>
-    <tableColumn id="6" name="L5" dataDxfId="65"/>
-    <tableColumn id="7" name="L6" dataDxfId="64"/>
-    <tableColumn id="8" name="L7" dataDxfId="63"/>
-    <tableColumn id="9" name="L8" dataDxfId="62"/>
-    <tableColumn id="10" name="L9" dataDxfId="61"/>
-    <tableColumn id="11" name="L10" dataDxfId="60"/>
+    <tableColumn id="1" name="Max Level" dataDxfId="72"/>
+    <tableColumn id="2" name="L1" dataDxfId="71"/>
+    <tableColumn id="3" name="L2" dataDxfId="70"/>
+    <tableColumn id="4" name="L3" dataDxfId="69"/>
+    <tableColumn id="5" name="L4" dataDxfId="68"/>
+    <tableColumn id="6" name="L5" dataDxfId="67"/>
+    <tableColumn id="7" name="L6" dataDxfId="66"/>
+    <tableColumn id="8" name="L7" dataDxfId="65"/>
+    <tableColumn id="9" name="L8" dataDxfId="64"/>
+    <tableColumn id="10" name="L9" dataDxfId="63"/>
+    <tableColumn id="11" name="L10" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HeroUpgrades" displayName="HeroUpgrades" ref="A56:E96" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HeroUpgrades" displayName="HeroUpgrades" ref="A56:E96" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" tableBorderDxfId="59">
   <autoFilter ref="A56:E96"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Level" dataDxfId="56"/>
-    <tableColumn id="2" name="BK-Cost" dataDxfId="55"/>
-    <tableColumn id="3" name="BK-Time" dataDxfId="54"/>
-    <tableColumn id="4" name="AQ-Cost" dataDxfId="53"/>
-    <tableColumn id="5" name="AQ-Time" dataDxfId="52"/>
+    <tableColumn id="1" name="Level" dataDxfId="58"/>
+    <tableColumn id="2" name="BK-Cost" dataDxfId="57"/>
+    <tableColumn id="3" name="BK-Time" dataDxfId="56"/>
+    <tableColumn id="4" name="AQ-Cost" dataDxfId="55"/>
+    <tableColumn id="5" name="AQ-Time" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A100:B108" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A100:B108" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <tableColumns count="2">
-    <tableColumn id="1" name="Level" dataDxfId="49"/>
-    <tableColumn id="2" name="Capacity" dataDxfId="48"/>
+    <tableColumn id="1" name="Level" dataDxfId="51"/>
+    <tableColumn id="2" name="Capacity" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8701,11 +8730,11 @@
   </sheetPr>
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="I11" sqref="I11:N11"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8871,7 +8900,7 @@
       </c>
       <c r="K6" s="20">
         <f ca="1">SUMIFS(CostRemaining[Sum],CostRemaining[Resource],K$5,CostRemaining[Kind],$I6)</f>
-        <v>1250000</v>
+        <v>5750000</v>
       </c>
       <c r="L6" s="20">
         <f ca="1">SUMIFS(CostRemaining[Sum],CostRemaining[Resource],L$5,CostRemaining[Kind],$I6)</f>
@@ -8879,11 +8908,11 @@
       </c>
       <c r="M6" s="152">
         <f ca="1">SUMIF(TimeRemaining[Kind],$I6,TimeRemaining[Sum])</f>
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="N6" s="127">
         <f ca="1">M6/IF(I6="Building",NumBuilders,1)</f>
-        <v>2.6</v>
+        <v>5</v>
       </c>
       <c r="O6" s="128"/>
       <c r="P6" s="18" t="s">
@@ -8916,7 +8945,7 @@
       </c>
       <c r="J7" s="23">
         <f ca="1">SUMIFS(CostRemaining[Sum],CostRemaining[Resource],J$5,CostRemaining[Kind],$I7)</f>
-        <v>43725000</v>
+        <v>41550000</v>
       </c>
       <c r="K7" s="157"/>
       <c r="L7" s="157"/>
@@ -9003,11 +9032,11 @@
       </c>
       <c r="J9" s="32">
         <f ca="1">SUM(J6:J8)</f>
-        <v>45725000</v>
+        <v>43550000</v>
       </c>
       <c r="K9" s="33">
         <f ca="1">SUM(K6:K8)</f>
-        <v>7300000</v>
+        <v>11800000</v>
       </c>
       <c r="L9" s="91">
         <f ca="1">SUM(L6:L8)</f>
@@ -9088,8 +9117,8 @@
       </c>
       <c r="M12" s="275"/>
       <c r="N12" s="190">
-        <f t="array" aca="1" ref="N12" ca="1">SUM(IF(ConstructionState[Kind]="Building",(ConstructionState[Available]*ConstructionState[Maximum Level])))-SUMPRODUCT(IF(ConstructionState[Kind]="Building",ConstructionState[[1]:[12]]*ConstructionState[[#Headers],[1]:[12]]))</f>
-        <v>7</v>
+        <f t="array" aca="1" ref="N12" ca="1">SUM(IF(COUNTIF(Skips,ConstructionState[Building or Upgrade])=0,IF(ConstructionState[Kind]="Building",(ConstructionState[Available]*ConstructionState[Maximum Level]))))-SUMPRODUCT(IF(COUNTIF(Skips,ConstructionState[Building or Upgrade])=0,IF(ConstructionState[Kind]="Building",ConstructionState[[1]:[12]]*ConstructionState[[#Headers],[1]:[12]])))</f>
+        <v>5</v>
       </c>
       <c r="O12" s="128"/>
       <c r="P12" s="12" t="s">
@@ -9129,8 +9158,8 @@
       </c>
       <c r="M13" s="279"/>
       <c r="N13" s="191">
-        <f t="array" aca="1" ref="N13" ca="1">SUM(IF(ConstructionState[Kind]="Wall",(ConstructionState[Available]*ConstructionState[Maximum Level])))-SUMPRODUCT(IF(ConstructionState[Kind]="Wall",ConstructionState[[1]:[12]]*ConstructionState[[#Headers],[1]:[12]]))</f>
-        <v>293</v>
+        <f t="array" aca="1" ref="N13" ca="1">SUM(IF(COUNTIF(Skips,ConstructionState[Building or Upgrade])=0,IF(ConstructionState[Kind]="Wall",(ConstructionState[Available]*ConstructionState[Maximum Level]))))-SUMPRODUCT(IF(COUNTIF(Skips,ConstructionState[Building or Upgrade])=0,IF(ConstructionState[Kind]="Wall",ConstructionState[[1]:[12]]*ConstructionState[[#Headers],[1]:[12]])))</f>
+        <v>264</v>
       </c>
       <c r="O13" s="128"/>
       <c r="P13" s="18" t="s">
@@ -9164,15 +9193,15 @@
       <c r="J14" s="277"/>
       <c r="K14" s="10">
         <f ca="1">K9/J9</f>
-        <v>0.15965008201202843</v>
+        <v>0.27095292766934559</v>
       </c>
       <c r="L14" s="280" t="s">
         <v>253</v>
       </c>
       <c r="M14" s="281"/>
       <c r="N14" s="192">
-        <f t="array" aca="1" ref="N14" ca="1">SUM(IF(ConstructionState[Kind]="Upgrade",(ConstructionState[Available]*ConstructionState[Maximum Level])))-SUMPRODUCT(IF(ConstructionState[Kind]="Upgrade",ConstructionState[[1]:[12]]*ConstructionState[[#Headers],[1]:[12]]))</f>
-        <v>11</v>
+        <f t="array" aca="1" ref="N14" ca="1">SUM(IF(COUNTIF(Skips,ConstructionState[Building or Upgrade])=0,IF(ConstructionState[Kind]="Upgrade",(ConstructionState[Available]*ConstructionState[Maximum Level]))))-SUMPRODUCT(IF(COUNTIF(Skips,ConstructionState[Building or Upgrade])=0,IF(ConstructionState[Kind]="Upgrade",ConstructionState[[1]:[12]]*ConstructionState[[#Headers],[1]:[12]])))</f>
+        <v>7</v>
       </c>
       <c r="O14" s="128"/>
       <c r="P14" s="27" t="s">
@@ -9323,9 +9352,7 @@
       <c r="Q19" s="174" t="s">
         <v>97</v>
       </c>
-      <c r="R19" s="174" t="s">
-        <v>2</v>
-      </c>
+      <c r="R19" s="174"/>
       <c r="S19" s="175" t="s">
         <v>18</v>
       </c>
@@ -9577,7 +9604,7 @@
       </c>
       <c r="D26" s="49" t="str">
         <f>IF(COUNTIF(Skips,ConstructionState[[#This Row],[Building or Upgrade]]),"IGNORE",ConstructionState[Kind]&amp;"-"&amp;ConstructionState[Resource])</f>
-        <v>IGNORE</v>
+        <v>Building-Elixir</v>
       </c>
       <c r="E26" s="50">
         <f ca="1">IF(AND(ConstructionState[[#This Row],[Kind]]="Upgrade",LabLevel=0),0,VLOOKUP(ConstructionState[Building or Upgrade],QuantAvail[],1+IF(ConstructionState[[#This Row],[Kind]]="Upgrade",LabLevel,THLevel),FALSE))</f>
@@ -9597,11 +9624,9 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="2">
-        <v>1</v>
-      </c>
+      <c r="N26" s="2"/>
       <c r="O26" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P26" s="4">
         <v>1</v>
@@ -10157,10 +10182,10 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="M39" s="2">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="N39" s="2">
         <v>1</v>
@@ -11620,33 +11645,33 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="J6:N6 Q6:S8 Q13:S14 I21:I22 K8:N8 J7">
-    <cfRule type="cellIs" dxfId="256" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I22">
-    <cfRule type="cellIs" dxfId="255" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="16" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:S72">
-    <cfRule type="expression" dxfId="254" priority="80">
+    <cfRule type="expression" dxfId="256" priority="80">
       <formula>OR(VALUE(H$23)&gt;$F24,AND($B24="Upgrade",H$23="1"))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="253" priority="81">
+    <cfRule type="expression" dxfId="255" priority="81">
       <formula>AND(VALUE(H$23)&lt;$F24,VALUE(H24)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsErrors" dxfId="252" priority="2">
+    <cfRule type="containsErrors" dxfId="254" priority="2">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24:G72">
-    <cfRule type="cellIs" dxfId="251" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="253" priority="54" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="252" priority="55" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11695,8 +11720,8 @@
   </sheetPr>
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
       <selection activeCell="M15" sqref="M15"/>
@@ -11808,25 +11833,25 @@
     </row>
     <row r="4" spans="1:25" ht="16" thickTop="1">
       <c r="A4" s="130"/>
-      <c r="B4" s="296" t="s">
+      <c r="B4" s="299" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="297"/>
-      <c r="D4" s="297"/>
-      <c r="E4" s="297"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="297"/>
-      <c r="H4" s="298"/>
+      <c r="C4" s="300"/>
+      <c r="D4" s="300"/>
+      <c r="E4" s="300"/>
+      <c r="F4" s="300"/>
+      <c r="G4" s="300"/>
+      <c r="H4" s="301"/>
       <c r="I4" s="130"/>
       <c r="J4" s="93">
         <v>2</v>
       </c>
-      <c r="K4" s="305" t="s">
+      <c r="K4" s="308" t="s">
         <v>176</v>
       </c>
-      <c r="L4" s="306"/>
-      <c r="M4" s="306"/>
-      <c r="N4" s="307"/>
+      <c r="L4" s="309"/>
+      <c r="M4" s="309"/>
+      <c r="N4" s="310"/>
       <c r="O4" s="130"/>
       <c r="P4" s="130"/>
       <c r="Q4" s="130"/>
@@ -11841,23 +11866,23 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="130"/>
-      <c r="B5" s="299"/>
-      <c r="C5" s="300"/>
-      <c r="D5" s="300"/>
-      <c r="E5" s="300"/>
-      <c r="F5" s="300"/>
-      <c r="G5" s="300"/>
-      <c r="H5" s="301"/>
+      <c r="B5" s="302"/>
+      <c r="C5" s="303"/>
+      <c r="D5" s="303"/>
+      <c r="E5" s="303"/>
+      <c r="F5" s="303"/>
+      <c r="G5" s="303"/>
+      <c r="H5" s="304"/>
       <c r="I5" s="130"/>
       <c r="J5" s="36">
         <v>0</v>
       </c>
-      <c r="K5" s="308" t="s">
+      <c r="K5" s="311" t="s">
         <v>177</v>
       </c>
-      <c r="L5" s="309"/>
-      <c r="M5" s="309"/>
-      <c r="N5" s="310"/>
+      <c r="L5" s="312"/>
+      <c r="M5" s="312"/>
+      <c r="N5" s="313"/>
       <c r="O5" s="130"/>
       <c r="P5" s="130"/>
       <c r="Q5" s="130"/>
@@ -11872,23 +11897,23 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="130"/>
-      <c r="B6" s="299"/>
-      <c r="C6" s="300"/>
-      <c r="D6" s="300"/>
-      <c r="E6" s="300"/>
-      <c r="F6" s="300"/>
-      <c r="G6" s="300"/>
-      <c r="H6" s="301"/>
+      <c r="B6" s="302"/>
+      <c r="C6" s="303"/>
+      <c r="D6" s="303"/>
+      <c r="E6" s="303"/>
+      <c r="F6" s="303"/>
+      <c r="G6" s="303"/>
+      <c r="H6" s="304"/>
       <c r="I6" s="130"/>
       <c r="J6" s="38">
         <v>-1</v>
       </c>
-      <c r="K6" s="308" t="s">
+      <c r="K6" s="311" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="309"/>
-      <c r="M6" s="309"/>
-      <c r="N6" s="310"/>
+      <c r="L6" s="312"/>
+      <c r="M6" s="312"/>
+      <c r="N6" s="313"/>
       <c r="O6" s="130"/>
       <c r="P6" s="130"/>
       <c r="Q6" s="130"/>
@@ -11903,21 +11928,21 @@
     </row>
     <row r="7" spans="1:25" ht="16" thickBot="1">
       <c r="A7" s="130"/>
-      <c r="B7" s="302"/>
-      <c r="C7" s="303"/>
-      <c r="D7" s="303"/>
-      <c r="E7" s="303"/>
-      <c r="F7" s="303"/>
-      <c r="G7" s="303"/>
-      <c r="H7" s="304"/>
+      <c r="B7" s="305"/>
+      <c r="C7" s="306"/>
+      <c r="D7" s="306"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="306"/>
+      <c r="G7" s="306"/>
+      <c r="H7" s="307"/>
       <c r="I7" s="130"/>
       <c r="J7" s="92"/>
-      <c r="K7" s="311" t="s">
+      <c r="K7" s="314" t="s">
         <v>159</v>
       </c>
-      <c r="L7" s="312"/>
-      <c r="M7" s="312"/>
-      <c r="N7" s="313"/>
+      <c r="L7" s="315"/>
+      <c r="M7" s="315"/>
+      <c r="N7" s="316"/>
       <c r="O7" s="130"/>
       <c r="P7" s="130"/>
       <c r="Q7" s="130"/>
@@ -11959,20 +11984,20 @@
     </row>
     <row r="9" spans="1:25" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="130"/>
-      <c r="B9" s="288" t="s">
+      <c r="B9" s="291" t="s">
         <v>175</v>
       </c>
       <c r="C9" s="219"/>
       <c r="D9" s="220"/>
       <c r="E9" s="130"/>
-      <c r="F9" s="288" t="s">
+      <c r="F9" s="291" t="s">
         <v>172</v>
       </c>
       <c r="G9" s="219"/>
       <c r="H9" s="219"/>
       <c r="I9" s="220"/>
       <c r="J9" s="130"/>
-      <c r="K9" s="288" t="s">
+      <c r="K9" s="291" t="s">
         <v>173</v>
       </c>
       <c r="L9" s="219"/>
@@ -12021,10 +12046,10 @@
       <c r="L10" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="289" t="s">
+      <c r="M10" s="292" t="s">
         <v>174</v>
       </c>
-      <c r="N10" s="290"/>
+      <c r="N10" s="293"/>
       <c r="O10" s="130"/>
       <c r="P10" s="130"/>
       <c r="Q10" s="130"/>
@@ -12074,11 +12099,11 @@
         <f>SUMIFS(ArmyState[Total Time],ArmyState[Type],"Unit",ArmyState[Resource],"Elixir")</f>
         <v>92.333333333333329</v>
       </c>
-      <c r="M11" s="291">
+      <c r="M11" s="294">
         <f ca="1">L11/NumBarracks</f>
         <v>23.083333333333332</v>
       </c>
-      <c r="N11" s="292"/>
+      <c r="N11" s="295"/>
       <c r="O11" s="130"/>
       <c r="P11" s="130"/>
       <c r="Q11" s="130"/>
@@ -12128,11 +12153,11 @@
         <f>SUMIFS(ArmyState[Total Time],ArmyState[Type],"Unit",ArmyState[Resource],"Dark Elixir")</f>
         <v>0</v>
       </c>
-      <c r="M12" s="293">
+      <c r="M12" s="296">
         <f ca="1">L12/NumDarkBarracks</f>
         <v>0</v>
       </c>
-      <c r="N12" s="292"/>
+      <c r="N12" s="295"/>
       <c r="O12" s="130"/>
       <c r="P12" s="130"/>
       <c r="Q12" s="130"/>
@@ -12171,11 +12196,11 @@
         <f>SUMIFS(ArmyState[Total Time],ArmyState[Type],"Spell")</f>
         <v>0</v>
       </c>
-      <c r="M13" s="294">
+      <c r="M13" s="297">
         <f>L13/1</f>
         <v>0</v>
       </c>
-      <c r="N13" s="295"/>
+      <c r="N13" s="298"/>
       <c r="O13" s="130"/>
       <c r="P13" s="130"/>
       <c r="Q13" s="130"/>
@@ -12217,35 +12242,35 @@
     </row>
     <row r="15" spans="1:25" ht="25" thickTop="1" thickBot="1">
       <c r="A15" s="130"/>
-      <c r="B15" s="282" t="s">
+      <c r="B15" s="285" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="283"/>
-      <c r="D15" s="334" t="s">
+      <c r="C15" s="286"/>
+      <c r="D15" s="282" t="s">
         <v>204</v>
       </c>
-      <c r="E15" s="335"/>
-      <c r="F15" s="335"/>
-      <c r="G15" s="336"/>
+      <c r="E15" s="283"/>
+      <c r="F15" s="283"/>
+      <c r="G15" s="284"/>
       <c r="H15" s="130"/>
       <c r="I15" s="130"/>
       <c r="J15" s="130"/>
       <c r="K15" s="130"/>
       <c r="L15" s="130"/>
       <c r="M15" s="130"/>
-      <c r="N15" s="284" t="s">
+      <c r="N15" s="287" t="s">
         <v>185</v>
       </c>
-      <c r="O15" s="285"/>
-      <c r="P15" s="286"/>
-      <c r="Q15" s="286"/>
-      <c r="R15" s="286"/>
-      <c r="S15" s="286"/>
-      <c r="T15" s="286"/>
-      <c r="U15" s="286"/>
-      <c r="V15" s="286"/>
-      <c r="W15" s="286"/>
-      <c r="X15" s="287"/>
+      <c r="O15" s="288"/>
+      <c r="P15" s="289"/>
+      <c r="Q15" s="289"/>
+      <c r="R15" s="289"/>
+      <c r="S15" s="289"/>
+      <c r="T15" s="289"/>
+      <c r="U15" s="289"/>
+      <c r="V15" s="289"/>
+      <c r="W15" s="289"/>
+      <c r="X15" s="290"/>
       <c r="Y15" s="130"/>
     </row>
     <row r="16" spans="1:25" ht="17" thickTop="1" thickBot="1">
@@ -13913,30 +13938,30 @@
     <mergeCell ref="K9:N9"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:D13 L11:M13 G11:I12 O38:X41">
-    <cfRule type="cellIs" dxfId="228" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I12">
-    <cfRule type="cellIs" dxfId="227" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="229" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="228" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:X17">
-    <cfRule type="expression" dxfId="225" priority="1">
+    <cfRule type="expression" dxfId="227" priority="1">
       <formula>$D$15=O$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsErrors" dxfId="224" priority="4">
+    <cfRule type="containsErrors" dxfId="226" priority="4">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:X37">
-    <cfRule type="expression" dxfId="223" priority="2">
+    <cfRule type="expression" dxfId="225" priority="2">
       <formula>$D$15=N$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13983,97 +14008,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickTop="1">
-      <c r="A1" s="314" t="s">
+      <c r="A1" s="317" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="315"/>
-      <c r="C1" s="315"/>
-      <c r="D1" s="315"/>
-      <c r="E1" s="315"/>
-      <c r="F1" s="316"/>
+      <c r="B1" s="318"/>
+      <c r="C1" s="318"/>
+      <c r="D1" s="318"/>
+      <c r="E1" s="318"/>
+      <c r="F1" s="319"/>
     </row>
     <row r="2" spans="1:6" ht="16" thickBot="1">
-      <c r="A2" s="317"/>
-      <c r="B2" s="318"/>
-      <c r="C2" s="318"/>
-      <c r="D2" s="318"/>
-      <c r="E2" s="318"/>
-      <c r="F2" s="319"/>
+      <c r="A2" s="320"/>
+      <c r="B2" s="321"/>
+      <c r="C2" s="321"/>
+      <c r="D2" s="321"/>
+      <c r="E2" s="321"/>
+      <c r="F2" s="322"/>
     </row>
     <row r="3" spans="1:6" ht="16" thickTop="1"/>
     <row r="4" spans="1:6">
-      <c r="A4" s="320" t="s">
+      <c r="A4" s="323" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="321"/>
-      <c r="C4" s="321"/>
-      <c r="D4" s="321"/>
-      <c r="E4" s="321"/>
-      <c r="F4" s="321"/>
+      <c r="B4" s="324"/>
+      <c r="C4" s="324"/>
+      <c r="D4" s="324"/>
+      <c r="E4" s="324"/>
+      <c r="F4" s="324"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="321"/>
-      <c r="B5" s="321"/>
-      <c r="C5" s="321"/>
-      <c r="D5" s="321"/>
-      <c r="E5" s="321"/>
-      <c r="F5" s="321"/>
+      <c r="A5" s="324"/>
+      <c r="B5" s="324"/>
+      <c r="C5" s="324"/>
+      <c r="D5" s="324"/>
+      <c r="E5" s="324"/>
+      <c r="F5" s="324"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="321"/>
-      <c r="B6" s="321"/>
-      <c r="C6" s="321"/>
-      <c r="D6" s="321"/>
-      <c r="E6" s="321"/>
-      <c r="F6" s="321"/>
+      <c r="A6" s="324"/>
+      <c r="B6" s="324"/>
+      <c r="C6" s="324"/>
+      <c r="D6" s="324"/>
+      <c r="E6" s="324"/>
+      <c r="F6" s="324"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="321"/>
-      <c r="B7" s="321"/>
-      <c r="C7" s="321"/>
-      <c r="D7" s="321"/>
-      <c r="E7" s="321"/>
-      <c r="F7" s="321"/>
+      <c r="A7" s="324"/>
+      <c r="B7" s="324"/>
+      <c r="C7" s="324"/>
+      <c r="D7" s="324"/>
+      <c r="E7" s="324"/>
+      <c r="F7" s="324"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="321"/>
-      <c r="B8" s="321"/>
-      <c r="C8" s="321"/>
-      <c r="D8" s="321"/>
-      <c r="E8" s="321"/>
-      <c r="F8" s="321"/>
+      <c r="A8" s="324"/>
+      <c r="B8" s="324"/>
+      <c r="C8" s="324"/>
+      <c r="D8" s="324"/>
+      <c r="E8" s="324"/>
+      <c r="F8" s="324"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="321"/>
-      <c r="B9" s="321"/>
-      <c r="C9" s="321"/>
-      <c r="D9" s="321"/>
-      <c r="E9" s="321"/>
-      <c r="F9" s="321"/>
+      <c r="A9" s="324"/>
+      <c r="B9" s="324"/>
+      <c r="C9" s="324"/>
+      <c r="D9" s="324"/>
+      <c r="E9" s="324"/>
+      <c r="F9" s="324"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="322"/>
-      <c r="B10" s="322"/>
-      <c r="C10" s="322"/>
-      <c r="D10" s="322"/>
-      <c r="E10" s="322"/>
-      <c r="F10" s="322"/>
+      <c r="A10" s="325"/>
+      <c r="B10" s="325"/>
+      <c r="C10" s="325"/>
+      <c r="D10" s="325"/>
+      <c r="E10" s="325"/>
+      <c r="F10" s="325"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="322"/>
-      <c r="B11" s="322"/>
-      <c r="C11" s="322"/>
-      <c r="D11" s="322"/>
-      <c r="E11" s="322"/>
-      <c r="F11" s="322"/>
+      <c r="A11" s="325"/>
+      <c r="B11" s="325"/>
+      <c r="C11" s="325"/>
+      <c r="D11" s="325"/>
+      <c r="E11" s="325"/>
+      <c r="F11" s="325"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="322"/>
-      <c r="B12" s="322"/>
-      <c r="C12" s="322"/>
-      <c r="D12" s="322"/>
-      <c r="E12" s="322"/>
-      <c r="F12" s="322"/>
+      <c r="A12" s="325"/>
+      <c r="B12" s="325"/>
+      <c r="C12" s="325"/>
+      <c r="D12" s="325"/>
+      <c r="E12" s="325"/>
+      <c r="F12" s="325"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -14101,8 +14126,8 @@
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
-    <sheetView topLeftCell="A29" workbookViewId="1">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14115,10 +14140,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="16" thickBot="1"/>
     <row r="2" spans="2:3" ht="17" thickTop="1" thickBot="1">
-      <c r="B2" s="323" t="s">
+      <c r="B2" s="326" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="324"/>
+      <c r="C2" s="327"/>
     </row>
     <row r="3" spans="2:3" ht="16" thickTop="1">
       <c r="B3" s="100"/>
@@ -14216,10 +14241,10 @@
       <c r="C19" s="35"/>
     </row>
     <row r="20" spans="2:3" ht="17" thickTop="1" thickBot="1">
-      <c r="B20" s="323" t="s">
+      <c r="B20" s="326" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="324"/>
+      <c r="C20" s="327"/>
     </row>
     <row r="21" spans="2:3" ht="16" thickTop="1">
       <c r="B21" s="100"/>
@@ -14235,10 +14260,10 @@
       <c r="B23" s="111"/>
     </row>
     <row r="24" spans="2:3" ht="17" thickTop="1" thickBot="1">
-      <c r="B24" s="323" t="s">
+      <c r="B24" s="326" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="324"/>
+      <c r="C24" s="327"/>
     </row>
     <row r="25" spans="2:3" ht="46" thickTop="1">
       <c r="B25" s="103"/>
@@ -14274,10 +14299,10 @@
       <c r="B30" s="111"/>
     </row>
     <row r="31" spans="2:3" ht="17" thickTop="1" thickBot="1">
-      <c r="B31" s="323" t="s">
+      <c r="B31" s="326" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="324"/>
+      <c r="C31" s="327"/>
     </row>
     <row r="32" spans="2:3" ht="16" thickTop="1">
       <c r="B32" s="170"/>
@@ -14309,10 +14334,10 @@
     </row>
     <row r="37" spans="1:3" ht="17" thickTop="1" thickBot="1"/>
     <row r="38" spans="1:3" ht="17" thickTop="1" thickBot="1">
-      <c r="B38" s="323" t="s">
+      <c r="B38" s="326" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="324"/>
+      <c r="C38" s="327"/>
     </row>
     <row r="39" spans="1:3" ht="16" thickTop="1">
       <c r="B39" s="163" t="s">
@@ -14378,8 +14403,12 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="111"/>
-      <c r="B46" s="114"/>
-      <c r="C46" s="112"/>
+      <c r="B46" s="114">
+        <v>41832</v>
+      </c>
+      <c r="C46" s="112" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="111"/>
@@ -14396,10 +14425,10 @@
     </row>
     <row r="50" spans="1:3" ht="17" thickTop="1" thickBot="1">
       <c r="A50" s="111"/>
-      <c r="B50" s="323" t="s">
+      <c r="B50" s="326" t="s">
         <v>141</v>
       </c>
-      <c r="C50" s="324"/>
+      <c r="C50" s="327"/>
     </row>
     <row r="51" spans="1:3" ht="16" thickTop="1">
       <c r="A51" s="111"/>
@@ -14506,35 +14535,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A1" s="328" t="s">
+      <c r="A1" s="331" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="329"/>
-      <c r="C1" s="329"/>
-      <c r="D1" s="329"/>
-      <c r="E1" s="329"/>
-      <c r="F1" s="329"/>
-      <c r="G1" s="329"/>
-      <c r="H1" s="329"/>
-      <c r="I1" s="329"/>
-      <c r="J1" s="329"/>
-      <c r="K1" s="329"/>
-      <c r="L1" s="329"/>
-      <c r="M1" s="329"/>
-      <c r="N1" s="329"/>
-      <c r="O1" s="329"/>
-      <c r="P1" s="329"/>
-      <c r="Q1" s="329"/>
-      <c r="R1" s="329"/>
-      <c r="S1" s="329"/>
-      <c r="T1" s="329"/>
-      <c r="U1" s="329"/>
-      <c r="V1" s="329"/>
-      <c r="W1" s="329"/>
-      <c r="X1" s="329"/>
-      <c r="Y1" s="329"/>
-      <c r="Z1" s="329"/>
-      <c r="AA1" s="330"/>
+      <c r="B1" s="332"/>
+      <c r="C1" s="332"/>
+      <c r="D1" s="332"/>
+      <c r="E1" s="332"/>
+      <c r="F1" s="332"/>
+      <c r="G1" s="332"/>
+      <c r="H1" s="332"/>
+      <c r="I1" s="332"/>
+      <c r="J1" s="332"/>
+      <c r="K1" s="332"/>
+      <c r="L1" s="332"/>
+      <c r="M1" s="332"/>
+      <c r="N1" s="332"/>
+      <c r="O1" s="332"/>
+      <c r="P1" s="332"/>
+      <c r="Q1" s="332"/>
+      <c r="R1" s="332"/>
+      <c r="S1" s="332"/>
+      <c r="T1" s="332"/>
+      <c r="U1" s="332"/>
+      <c r="V1" s="332"/>
+      <c r="W1" s="332"/>
+      <c r="X1" s="332"/>
+      <c r="Y1" s="332"/>
+      <c r="Z1" s="332"/>
+      <c r="AA1" s="333"/>
     </row>
     <row r="2" spans="1:27" ht="16" customHeight="1" thickTop="1">
       <c r="A2" s="11" t="s">
@@ -18716,35 +18745,35 @@
       <c r="AA52" s="77"/>
     </row>
     <row r="53" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A53" s="325" t="s">
+      <c r="A53" s="328" t="s">
         <v>208</v>
       </c>
-      <c r="B53" s="326"/>
-      <c r="C53" s="326"/>
-      <c r="D53" s="326"/>
-      <c r="E53" s="326"/>
-      <c r="F53" s="326"/>
-      <c r="G53" s="326"/>
-      <c r="H53" s="326"/>
-      <c r="I53" s="326"/>
-      <c r="J53" s="326"/>
-      <c r="K53" s="326"/>
-      <c r="L53" s="326"/>
-      <c r="M53" s="326"/>
-      <c r="N53" s="326"/>
-      <c r="O53" s="326"/>
-      <c r="P53" s="326"/>
-      <c r="Q53" s="326"/>
-      <c r="R53" s="326"/>
-      <c r="S53" s="326"/>
-      <c r="T53" s="326"/>
-      <c r="U53" s="326"/>
-      <c r="V53" s="326"/>
-      <c r="W53" s="326"/>
-      <c r="X53" s="326"/>
-      <c r="Y53" s="326"/>
-      <c r="Z53" s="326"/>
-      <c r="AA53" s="327"/>
+      <c r="B53" s="329"/>
+      <c r="C53" s="329"/>
+      <c r="D53" s="329"/>
+      <c r="E53" s="329"/>
+      <c r="F53" s="329"/>
+      <c r="G53" s="329"/>
+      <c r="H53" s="329"/>
+      <c r="I53" s="329"/>
+      <c r="J53" s="329"/>
+      <c r="K53" s="329"/>
+      <c r="L53" s="329"/>
+      <c r="M53" s="329"/>
+      <c r="N53" s="329"/>
+      <c r="O53" s="329"/>
+      <c r="P53" s="329"/>
+      <c r="Q53" s="329"/>
+      <c r="R53" s="329"/>
+      <c r="S53" s="329"/>
+      <c r="T53" s="329"/>
+      <c r="U53" s="329"/>
+      <c r="V53" s="329"/>
+      <c r="W53" s="329"/>
+      <c r="X53" s="329"/>
+      <c r="Y53" s="329"/>
+      <c r="Z53" s="329"/>
+      <c r="AA53" s="330"/>
     </row>
     <row r="54" spans="1:27" ht="17" thickTop="1" thickBot="1">
       <c r="A54" s="57"/>
@@ -18776,13 +18805,13 @@
       <c r="AA54" s="77"/>
     </row>
     <row r="55" spans="1:27" ht="19" thickTop="1">
-      <c r="A55" s="331" t="s">
+      <c r="A55" s="334" t="s">
         <v>224</v>
       </c>
-      <c r="B55" s="332"/>
-      <c r="C55" s="332"/>
-      <c r="D55" s="332"/>
-      <c r="E55" s="333"/>
+      <c r="B55" s="335"/>
+      <c r="C55" s="335"/>
+      <c r="D55" s="335"/>
+      <c r="E55" s="336"/>
       <c r="H55" s="75"/>
       <c r="I55" s="75"/>
       <c r="J55" s="75"/>
@@ -20069,35 +20098,35 @@
     </row>
     <row r="97" spans="1:27" ht="16" thickBot="1"/>
     <row r="98" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A98" s="325" t="s">
+      <c r="A98" s="328" t="s">
         <v>156</v>
       </c>
-      <c r="B98" s="326"/>
-      <c r="C98" s="326"/>
-      <c r="D98" s="326"/>
-      <c r="E98" s="326"/>
-      <c r="F98" s="326"/>
-      <c r="G98" s="326"/>
-      <c r="H98" s="326"/>
-      <c r="I98" s="326"/>
-      <c r="J98" s="326"/>
-      <c r="K98" s="326"/>
-      <c r="L98" s="326"/>
-      <c r="M98" s="326"/>
-      <c r="N98" s="326"/>
-      <c r="O98" s="326"/>
-      <c r="P98" s="326"/>
-      <c r="Q98" s="326"/>
-      <c r="R98" s="326"/>
-      <c r="S98" s="326"/>
-      <c r="T98" s="326"/>
-      <c r="U98" s="326"/>
-      <c r="V98" s="326"/>
-      <c r="W98" s="326"/>
-      <c r="X98" s="326"/>
-      <c r="Y98" s="326"/>
-      <c r="Z98" s="326"/>
-      <c r="AA98" s="327"/>
+      <c r="B98" s="329"/>
+      <c r="C98" s="329"/>
+      <c r="D98" s="329"/>
+      <c r="E98" s="329"/>
+      <c r="F98" s="329"/>
+      <c r="G98" s="329"/>
+      <c r="H98" s="329"/>
+      <c r="I98" s="329"/>
+      <c r="J98" s="329"/>
+      <c r="K98" s="329"/>
+      <c r="L98" s="329"/>
+      <c r="M98" s="329"/>
+      <c r="N98" s="329"/>
+      <c r="O98" s="329"/>
+      <c r="P98" s="329"/>
+      <c r="Q98" s="329"/>
+      <c r="R98" s="329"/>
+      <c r="S98" s="329"/>
+      <c r="T98" s="329"/>
+      <c r="U98" s="329"/>
+      <c r="V98" s="329"/>
+      <c r="W98" s="329"/>
+      <c r="X98" s="329"/>
+      <c r="Y98" s="329"/>
+      <c r="Z98" s="329"/>
+      <c r="AA98" s="330"/>
     </row>
     <row r="99" spans="1:27" ht="16" thickTop="1"/>
     <row r="100" spans="1:27">
@@ -20174,35 +20203,35 @@
     </row>
     <row r="109" spans="1:27" ht="16" thickBot="1"/>
     <row r="110" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A110" s="328" t="s">
+      <c r="A110" s="331" t="s">
         <v>155</v>
       </c>
-      <c r="B110" s="329"/>
-      <c r="C110" s="329"/>
-      <c r="D110" s="329"/>
-      <c r="E110" s="329"/>
-      <c r="F110" s="329"/>
-      <c r="G110" s="329"/>
-      <c r="H110" s="329"/>
-      <c r="I110" s="329"/>
-      <c r="J110" s="329"/>
-      <c r="K110" s="329"/>
-      <c r="L110" s="329"/>
-      <c r="M110" s="329"/>
-      <c r="N110" s="329"/>
-      <c r="O110" s="329"/>
-      <c r="P110" s="329"/>
-      <c r="Q110" s="329"/>
-      <c r="R110" s="329"/>
-      <c r="S110" s="329"/>
-      <c r="T110" s="329"/>
-      <c r="U110" s="329"/>
-      <c r="V110" s="329"/>
-      <c r="W110" s="329"/>
-      <c r="X110" s="329"/>
-      <c r="Y110" s="329"/>
-      <c r="Z110" s="329"/>
-      <c r="AA110" s="330"/>
+      <c r="B110" s="332"/>
+      <c r="C110" s="332"/>
+      <c r="D110" s="332"/>
+      <c r="E110" s="332"/>
+      <c r="F110" s="332"/>
+      <c r="G110" s="332"/>
+      <c r="H110" s="332"/>
+      <c r="I110" s="332"/>
+      <c r="J110" s="332"/>
+      <c r="K110" s="332"/>
+      <c r="L110" s="332"/>
+      <c r="M110" s="332"/>
+      <c r="N110" s="332"/>
+      <c r="O110" s="332"/>
+      <c r="P110" s="332"/>
+      <c r="Q110" s="332"/>
+      <c r="R110" s="332"/>
+      <c r="S110" s="332"/>
+      <c r="T110" s="332"/>
+      <c r="U110" s="332"/>
+      <c r="V110" s="332"/>
+      <c r="W110" s="332"/>
+      <c r="X110" s="332"/>
+      <c r="Y110" s="332"/>
+      <c r="Z110" s="332"/>
+      <c r="AA110" s="333"/>
     </row>
     <row r="111" spans="1:27" ht="16" thickTop="1">
       <c r="A111" s="11" t="s">
@@ -20941,35 +20970,35 @@
     </row>
     <row r="133" spans="1:27" ht="16" thickBot="1"/>
     <row r="134" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A134" s="325" t="s">
+      <c r="A134" s="328" t="s">
         <v>103</v>
       </c>
-      <c r="B134" s="326"/>
-      <c r="C134" s="326"/>
-      <c r="D134" s="326"/>
-      <c r="E134" s="326"/>
-      <c r="F134" s="326"/>
-      <c r="G134" s="326"/>
-      <c r="H134" s="326"/>
-      <c r="I134" s="326"/>
-      <c r="J134" s="326"/>
-      <c r="K134" s="326"/>
-      <c r="L134" s="326"/>
-      <c r="M134" s="326"/>
-      <c r="N134" s="326"/>
-      <c r="O134" s="326"/>
-      <c r="P134" s="326"/>
-      <c r="Q134" s="326"/>
-      <c r="R134" s="326"/>
-      <c r="S134" s="326"/>
-      <c r="T134" s="326"/>
-      <c r="U134" s="326"/>
-      <c r="V134" s="326"/>
-      <c r="W134" s="326"/>
-      <c r="X134" s="326"/>
-      <c r="Y134" s="326"/>
-      <c r="Z134" s="326"/>
-      <c r="AA134" s="327"/>
+      <c r="B134" s="329"/>
+      <c r="C134" s="329"/>
+      <c r="D134" s="329"/>
+      <c r="E134" s="329"/>
+      <c r="F134" s="329"/>
+      <c r="G134" s="329"/>
+      <c r="H134" s="329"/>
+      <c r="I134" s="329"/>
+      <c r="J134" s="329"/>
+      <c r="K134" s="329"/>
+      <c r="L134" s="329"/>
+      <c r="M134" s="329"/>
+      <c r="N134" s="329"/>
+      <c r="O134" s="329"/>
+      <c r="P134" s="329"/>
+      <c r="Q134" s="329"/>
+      <c r="R134" s="329"/>
+      <c r="S134" s="329"/>
+      <c r="T134" s="329"/>
+      <c r="U134" s="329"/>
+      <c r="V134" s="329"/>
+      <c r="W134" s="329"/>
+      <c r="X134" s="329"/>
+      <c r="Y134" s="329"/>
+      <c r="Z134" s="329"/>
+      <c r="AA134" s="330"/>
     </row>
     <row r="135" spans="1:27" ht="16" thickTop="1">
       <c r="A135" s="11" t="s">
@@ -22793,35 +22822,35 @@
     </row>
     <row r="187" spans="1:27" ht="16" thickBot="1"/>
     <row r="188" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A188" s="325" t="s">
+      <c r="A188" s="328" t="s">
         <v>127</v>
       </c>
-      <c r="B188" s="326"/>
-      <c r="C188" s="326"/>
-      <c r="D188" s="326"/>
-      <c r="E188" s="326"/>
-      <c r="F188" s="326"/>
-      <c r="G188" s="326"/>
-      <c r="H188" s="326"/>
-      <c r="I188" s="326"/>
-      <c r="J188" s="326"/>
-      <c r="K188" s="326"/>
-      <c r="L188" s="326"/>
-      <c r="M188" s="326"/>
-      <c r="N188" s="326"/>
-      <c r="O188" s="326"/>
-      <c r="P188" s="326"/>
-      <c r="Q188" s="326"/>
-      <c r="R188" s="326"/>
-      <c r="S188" s="326"/>
-      <c r="T188" s="326"/>
-      <c r="U188" s="326"/>
-      <c r="V188" s="326"/>
-      <c r="W188" s="326"/>
-      <c r="X188" s="326"/>
-      <c r="Y188" s="326"/>
-      <c r="Z188" s="326"/>
-      <c r="AA188" s="327"/>
+      <c r="B188" s="329"/>
+      <c r="C188" s="329"/>
+      <c r="D188" s="329"/>
+      <c r="E188" s="329"/>
+      <c r="F188" s="329"/>
+      <c r="G188" s="329"/>
+      <c r="H188" s="329"/>
+      <c r="I188" s="329"/>
+      <c r="J188" s="329"/>
+      <c r="K188" s="329"/>
+      <c r="L188" s="329"/>
+      <c r="M188" s="329"/>
+      <c r="N188" s="329"/>
+      <c r="O188" s="329"/>
+      <c r="P188" s="329"/>
+      <c r="Q188" s="329"/>
+      <c r="R188" s="329"/>
+      <c r="S188" s="329"/>
+      <c r="T188" s="329"/>
+      <c r="U188" s="329"/>
+      <c r="V188" s="329"/>
+      <c r="W188" s="329"/>
+      <c r="X188" s="329"/>
+      <c r="Y188" s="329"/>
+      <c r="Z188" s="329"/>
+      <c r="AA188" s="330"/>
     </row>
     <row r="189" spans="1:27" ht="16" thickTop="1">
       <c r="A189" s="11" t="s">
@@ -24645,35 +24674,35 @@
     </row>
     <row r="242" spans="1:27" ht="16" thickBot="1"/>
     <row r="243" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A243" s="325" t="s">
+      <c r="A243" s="328" t="s">
         <v>225</v>
       </c>
-      <c r="B243" s="326"/>
-      <c r="C243" s="326"/>
-      <c r="D243" s="326"/>
-      <c r="E243" s="326"/>
-      <c r="F243" s="326"/>
-      <c r="G243" s="326"/>
-      <c r="H243" s="326"/>
-      <c r="I243" s="326"/>
-      <c r="J243" s="326"/>
-      <c r="K243" s="326"/>
-      <c r="L243" s="326"/>
-      <c r="M243" s="326"/>
-      <c r="N243" s="326"/>
-      <c r="O243" s="326"/>
-      <c r="P243" s="326"/>
-      <c r="Q243" s="326"/>
-      <c r="R243" s="326"/>
-      <c r="S243" s="326"/>
-      <c r="T243" s="326"/>
-      <c r="U243" s="326"/>
-      <c r="V243" s="326"/>
-      <c r="W243" s="326"/>
-      <c r="X243" s="326"/>
-      <c r="Y243" s="326"/>
-      <c r="Z243" s="326"/>
-      <c r="AA243" s="327"/>
+      <c r="B243" s="329"/>
+      <c r="C243" s="329"/>
+      <c r="D243" s="329"/>
+      <c r="E243" s="329"/>
+      <c r="F243" s="329"/>
+      <c r="G243" s="329"/>
+      <c r="H243" s="329"/>
+      <c r="I243" s="329"/>
+      <c r="J243" s="329"/>
+      <c r="K243" s="329"/>
+      <c r="L243" s="329"/>
+      <c r="M243" s="329"/>
+      <c r="N243" s="329"/>
+      <c r="O243" s="329"/>
+      <c r="P243" s="329"/>
+      <c r="Q243" s="329"/>
+      <c r="R243" s="329"/>
+      <c r="S243" s="329"/>
+      <c r="T243" s="329"/>
+      <c r="U243" s="329"/>
+      <c r="V243" s="329"/>
+      <c r="W243" s="329"/>
+      <c r="X243" s="329"/>
+      <c r="Y243" s="329"/>
+      <c r="Z243" s="329"/>
+      <c r="AA243" s="330"/>
     </row>
     <row r="244" spans="1:27" ht="20" thickTop="1" thickBot="1">
       <c r="A244" s="94" t="s">
@@ -24976,277 +25005,277 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="D3:AA52 J65:T96 D56:D96 H55:I96 D54:AA54 J55:X64">
-    <cfRule type="containsErrors" dxfId="182" priority="61">
+    <cfRule type="containsErrors" dxfId="184" priority="61">
       <formula>ISERROR(D3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23:W23 P22:Q22 T22 P27:W27 P24:T26 P28:T29 P21:W21 P20:U20 P16:AA17 P15:V15 P19:X19 P18:Z18 P32:T52 P30:P31">
-    <cfRule type="containsErrors" dxfId="181" priority="60">
+    <cfRule type="containsErrors" dxfId="183" priority="60">
       <formula>ISERROR(P15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11:T11 P10:U10 P8:Z8 P7:U7">
-    <cfRule type="containsErrors" dxfId="180" priority="59">
+    <cfRule type="containsErrors" dxfId="182" priority="59">
       <formula>ISERROR(P7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:AA6">
-    <cfRule type="containsErrors" dxfId="179" priority="56">
+    <cfRule type="containsErrors" dxfId="181" priority="56">
       <formula>ISERROR(P6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:N9">
-    <cfRule type="containsErrors" dxfId="178" priority="55">
+    <cfRule type="containsErrors" dxfId="180" priority="55">
       <formula>ISERROR(D9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9:Z9">
-    <cfRule type="containsErrors" dxfId="177" priority="54">
+    <cfRule type="containsErrors" dxfId="179" priority="54">
       <formula>ISERROR(P9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsErrors" dxfId="176" priority="53">
+    <cfRule type="containsErrors" dxfId="178" priority="53">
       <formula>ISERROR(E41)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33">
-    <cfRule type="containsErrors" dxfId="175" priority="52">
+    <cfRule type="containsErrors" dxfId="177" priority="52">
       <formula>ISERROR(J33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:I41">
-    <cfRule type="containsErrors" dxfId="174" priority="51">
+    <cfRule type="containsErrors" dxfId="176" priority="51">
       <formula>ISERROR(I39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39:J41">
-    <cfRule type="containsErrors" dxfId="173" priority="50">
+    <cfRule type="containsErrors" dxfId="175" priority="50">
       <formula>ISERROR(J39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:K38 K42:K46">
-    <cfRule type="containsErrors" dxfId="172" priority="49">
+    <cfRule type="containsErrors" dxfId="174" priority="49">
       <formula>ISERROR(K34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33">
-    <cfRule type="containsErrors" dxfId="171" priority="48">
+    <cfRule type="containsErrors" dxfId="173" priority="48">
       <formula>ISERROR(K33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:K41">
-    <cfRule type="containsErrors" dxfId="170" priority="47">
+    <cfRule type="containsErrors" dxfId="172" priority="47">
       <formula>ISERROR(K39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L34:L38 L42:L46">
-    <cfRule type="containsErrors" dxfId="169" priority="46">
+    <cfRule type="containsErrors" dxfId="171" priority="46">
       <formula>ISERROR(L34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33">
-    <cfRule type="containsErrors" dxfId="168" priority="45">
+    <cfRule type="containsErrors" dxfId="170" priority="45">
       <formula>ISERROR(L33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39:L41">
-    <cfRule type="containsErrors" dxfId="167" priority="44">
+    <cfRule type="containsErrors" dxfId="169" priority="44">
       <formula>ISERROR(L39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34:M38 M42:M46">
-    <cfRule type="containsErrors" dxfId="166" priority="43">
+    <cfRule type="containsErrors" dxfId="168" priority="43">
       <formula>ISERROR(M34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M33">
-    <cfRule type="containsErrors" dxfId="165" priority="42">
+    <cfRule type="containsErrors" dxfId="167" priority="42">
       <formula>ISERROR(M33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M39:M41">
-    <cfRule type="containsErrors" dxfId="164" priority="41">
+    <cfRule type="containsErrors" dxfId="166" priority="41">
       <formula>ISERROR(M39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34:N38 N42:N46">
-    <cfRule type="containsErrors" dxfId="163" priority="40">
+    <cfRule type="containsErrors" dxfId="165" priority="40">
       <formula>ISERROR(N34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N33">
-    <cfRule type="containsErrors" dxfId="162" priority="39">
+    <cfRule type="containsErrors" dxfId="164" priority="39">
       <formula>ISERROR(N33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N39:N41">
-    <cfRule type="containsErrors" dxfId="161" priority="38">
+    <cfRule type="containsErrors" dxfId="163" priority="38">
       <formula>ISERROR(N39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O34:O38 O42:O46">
-    <cfRule type="containsErrors" dxfId="160" priority="37">
+    <cfRule type="containsErrors" dxfId="162" priority="37">
       <formula>ISERROR(O34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O33">
-    <cfRule type="containsErrors" dxfId="159" priority="36">
+    <cfRule type="containsErrors" dxfId="161" priority="36">
       <formula>ISERROR(O33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O39:O41">
-    <cfRule type="containsErrors" dxfId="158" priority="35">
+    <cfRule type="containsErrors" dxfId="160" priority="35">
       <formula>ISERROR(O39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W33:W52">
-    <cfRule type="containsErrors" dxfId="157" priority="34">
+    <cfRule type="containsErrors" dxfId="159" priority="34">
       <formula>ISERROR(W33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X33:X52">
-    <cfRule type="containsErrors" dxfId="156" priority="33">
+    <cfRule type="containsErrors" dxfId="158" priority="33">
       <formula>ISERROR(X33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y33:Y52">
-    <cfRule type="containsErrors" dxfId="155" priority="32">
+    <cfRule type="containsErrors" dxfId="157" priority="32">
       <formula>ISERROR(Y33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z33:Z52">
-    <cfRule type="containsErrors" dxfId="154" priority="31">
+    <cfRule type="containsErrors" dxfId="156" priority="31">
       <formula>ISERROR(Z33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA33:AA52">
-    <cfRule type="containsErrors" dxfId="153" priority="30">
+    <cfRule type="containsErrors" dxfId="155" priority="30">
       <formula>ISERROR(AA33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="containsErrors" dxfId="152" priority="28">
+    <cfRule type="containsErrors" dxfId="154" priority="28">
       <formula>ISERROR(D41)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D40 D42:D52 D54 D56:D96">
-    <cfRule type="containsErrors" dxfId="151" priority="29">
+    <cfRule type="containsErrors" dxfId="153" priority="29">
       <formula>ISERROR(D32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q30:R31">
-    <cfRule type="containsErrors" dxfId="150" priority="27">
+    <cfRule type="containsErrors" dxfId="152" priority="27">
       <formula>ISERROR(Q30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J120">
-    <cfRule type="containsErrors" dxfId="149" priority="26">
+    <cfRule type="containsErrors" dxfId="151" priority="26">
       <formula>ISERROR(J120)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J120">
-    <cfRule type="containsErrors" dxfId="148" priority="25">
+    <cfRule type="containsErrors" dxfId="150" priority="25">
       <formula>ISERROR(J120)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H131">
-    <cfRule type="containsErrors" dxfId="147" priority="4">
+    <cfRule type="containsErrors" dxfId="149" priority="4">
       <formula>ISERROR(H131)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126">
-    <cfRule type="containsErrors" dxfId="146" priority="3">
+    <cfRule type="containsErrors" dxfId="148" priority="3">
       <formula>ISERROR(K126)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J119">
-    <cfRule type="containsErrors" dxfId="145" priority="22">
+    <cfRule type="containsErrors" dxfId="147" priority="22">
       <formula>ISERROR(J119)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K119">
-    <cfRule type="containsErrors" dxfId="144" priority="20">
+    <cfRule type="containsErrors" dxfId="146" priority="20">
       <formula>ISERROR(K119)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K120">
-    <cfRule type="containsErrors" dxfId="143" priority="19">
+    <cfRule type="containsErrors" dxfId="145" priority="19">
       <formula>ISERROR(K120)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K121">
-    <cfRule type="containsErrors" dxfId="142" priority="18">
+    <cfRule type="containsErrors" dxfId="144" priority="18">
       <formula>ISERROR(K121)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J121">
-    <cfRule type="containsErrors" dxfId="141" priority="17">
+    <cfRule type="containsErrors" dxfId="143" priority="17">
       <formula>ISERROR(J121)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="containsErrors" dxfId="140" priority="16">
+    <cfRule type="containsErrors" dxfId="142" priority="16">
       <formula>ISERROR(K124)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K125">
-    <cfRule type="containsErrors" dxfId="139" priority="15">
+    <cfRule type="containsErrors" dxfId="141" priority="15">
       <formula>ISERROR(K125)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125">
-    <cfRule type="containsErrors" dxfId="138" priority="14">
+    <cfRule type="containsErrors" dxfId="140" priority="14">
       <formula>ISERROR(J125)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I125">
-    <cfRule type="containsErrors" dxfId="137" priority="13">
+    <cfRule type="containsErrors" dxfId="139" priority="13">
       <formula>ISERROR(I125)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H125">
-    <cfRule type="containsErrors" dxfId="136" priority="12">
+    <cfRule type="containsErrors" dxfId="138" priority="12">
       <formula>ISERROR(H125)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K128">
-    <cfRule type="containsErrors" dxfId="135" priority="11">
+    <cfRule type="containsErrors" dxfId="137" priority="11">
       <formula>ISERROR(K128)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129">
-    <cfRule type="containsErrors" dxfId="134" priority="10">
+    <cfRule type="containsErrors" dxfId="136" priority="10">
       <formula>ISERROR(K129)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J129">
-    <cfRule type="containsErrors" dxfId="133" priority="9">
+    <cfRule type="containsErrors" dxfId="135" priority="9">
       <formula>ISERROR(J129)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K130">
-    <cfRule type="containsErrors" dxfId="132" priority="8">
+    <cfRule type="containsErrors" dxfId="134" priority="8">
       <formula>ISERROR(K130)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K131">
-    <cfRule type="containsErrors" dxfId="131" priority="7">
+    <cfRule type="containsErrors" dxfId="133" priority="7">
       <formula>ISERROR(K131)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J131">
-    <cfRule type="containsErrors" dxfId="130" priority="6">
+    <cfRule type="containsErrors" dxfId="132" priority="6">
       <formula>ISERROR(J131)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I131">
-    <cfRule type="containsErrors" dxfId="129" priority="5">
+    <cfRule type="containsErrors" dxfId="131" priority="5">
       <formula>ISERROR(I131)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B190:K240 B136:K186">
-    <cfRule type="cellIs" dxfId="128" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25285,8 +25314,8 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A78" sqref="A78"/>
     </sheetView>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="1">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="1">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25298,35 +25327,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A1" s="325" t="s">
+      <c r="A1" s="328" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="326"/>
-      <c r="C1" s="326"/>
-      <c r="D1" s="326"/>
-      <c r="E1" s="326"/>
-      <c r="F1" s="326"/>
-      <c r="G1" s="326"/>
-      <c r="H1" s="326"/>
-      <c r="I1" s="326"/>
-      <c r="J1" s="326"/>
-      <c r="K1" s="326"/>
-      <c r="L1" s="326"/>
-      <c r="M1" s="326"/>
-      <c r="N1" s="326"/>
-      <c r="O1" s="326"/>
-      <c r="P1" s="326"/>
-      <c r="Q1" s="326"/>
-      <c r="R1" s="326"/>
-      <c r="S1" s="326"/>
-      <c r="T1" s="326"/>
-      <c r="U1" s="326"/>
-      <c r="V1" s="326"/>
-      <c r="W1" s="326"/>
-      <c r="X1" s="326"/>
-      <c r="Y1" s="326"/>
-      <c r="Z1" s="326"/>
-      <c r="AA1" s="327"/>
+      <c r="B1" s="329"/>
+      <c r="C1" s="329"/>
+      <c r="D1" s="329"/>
+      <c r="E1" s="329"/>
+      <c r="F1" s="329"/>
+      <c r="G1" s="329"/>
+      <c r="H1" s="329"/>
+      <c r="I1" s="329"/>
+      <c r="J1" s="329"/>
+      <c r="K1" s="329"/>
+      <c r="L1" s="329"/>
+      <c r="M1" s="329"/>
+      <c r="N1" s="329"/>
+      <c r="O1" s="329"/>
+      <c r="P1" s="329"/>
+      <c r="Q1" s="329"/>
+      <c r="R1" s="329"/>
+      <c r="S1" s="329"/>
+      <c r="T1" s="329"/>
+      <c r="U1" s="329"/>
+      <c r="V1" s="329"/>
+      <c r="W1" s="329"/>
+      <c r="X1" s="329"/>
+      <c r="Y1" s="329"/>
+      <c r="Z1" s="329"/>
+      <c r="AA1" s="330"/>
     </row>
     <row r="2" spans="1:27" ht="17" thickTop="1" thickBot="1"/>
     <row r="3" spans="1:27" ht="17" thickTop="1" thickBot="1">
@@ -25393,35 +25422,35 @@
     </row>
     <row r="10" spans="1:27" ht="17" thickTop="1" thickBot="1"/>
     <row r="11" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A11" s="325" t="s">
+      <c r="A11" s="328" t="s">
         <v>213</v>
       </c>
-      <c r="B11" s="326"/>
-      <c r="C11" s="326"/>
-      <c r="D11" s="326"/>
-      <c r="E11" s="326"/>
-      <c r="F11" s="326"/>
-      <c r="G11" s="326"/>
-      <c r="H11" s="326"/>
-      <c r="I11" s="326"/>
-      <c r="J11" s="326"/>
-      <c r="K11" s="326"/>
-      <c r="L11" s="326"/>
-      <c r="M11" s="326"/>
-      <c r="N11" s="326"/>
-      <c r="O11" s="326"/>
-      <c r="P11" s="326"/>
-      <c r="Q11" s="326"/>
-      <c r="R11" s="326"/>
-      <c r="S11" s="326"/>
-      <c r="T11" s="326"/>
-      <c r="U11" s="326"/>
-      <c r="V11" s="326"/>
-      <c r="W11" s="326"/>
-      <c r="X11" s="326"/>
-      <c r="Y11" s="326"/>
-      <c r="Z11" s="326"/>
-      <c r="AA11" s="327"/>
+      <c r="B11" s="329"/>
+      <c r="C11" s="329"/>
+      <c r="D11" s="329"/>
+      <c r="E11" s="329"/>
+      <c r="F11" s="329"/>
+      <c r="G11" s="329"/>
+      <c r="H11" s="329"/>
+      <c r="I11" s="329"/>
+      <c r="J11" s="329"/>
+      <c r="K11" s="329"/>
+      <c r="L11" s="329"/>
+      <c r="M11" s="329"/>
+      <c r="N11" s="329"/>
+      <c r="O11" s="329"/>
+      <c r="P11" s="329"/>
+      <c r="Q11" s="329"/>
+      <c r="R11" s="329"/>
+      <c r="S11" s="329"/>
+      <c r="T11" s="329"/>
+      <c r="U11" s="329"/>
+      <c r="V11" s="329"/>
+      <c r="W11" s="329"/>
+      <c r="X11" s="329"/>
+      <c r="Y11" s="329"/>
+      <c r="Z11" s="329"/>
+      <c r="AA11" s="330"/>
     </row>
     <row r="12" spans="1:27" ht="16" thickTop="1"/>
     <row r="13" spans="1:27">
@@ -25538,35 +25567,35 @@
     </row>
     <row r="16" spans="1:27" ht="16" thickBot="1"/>
     <row r="17" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A17" s="325" t="s">
+      <c r="A17" s="328" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="326"/>
-      <c r="C17" s="326"/>
-      <c r="D17" s="326"/>
-      <c r="E17" s="326"/>
-      <c r="F17" s="326"/>
-      <c r="G17" s="326"/>
-      <c r="H17" s="326"/>
-      <c r="I17" s="326"/>
-      <c r="J17" s="326"/>
-      <c r="K17" s="326"/>
-      <c r="L17" s="326"/>
-      <c r="M17" s="326"/>
-      <c r="N17" s="326"/>
-      <c r="O17" s="326"/>
-      <c r="P17" s="326"/>
-      <c r="Q17" s="326"/>
-      <c r="R17" s="326"/>
-      <c r="S17" s="326"/>
-      <c r="T17" s="326"/>
-      <c r="U17" s="326"/>
-      <c r="V17" s="326"/>
-      <c r="W17" s="326"/>
-      <c r="X17" s="326"/>
-      <c r="Y17" s="326"/>
-      <c r="Z17" s="326"/>
-      <c r="AA17" s="327"/>
+      <c r="B17" s="329"/>
+      <c r="C17" s="329"/>
+      <c r="D17" s="329"/>
+      <c r="E17" s="329"/>
+      <c r="F17" s="329"/>
+      <c r="G17" s="329"/>
+      <c r="H17" s="329"/>
+      <c r="I17" s="329"/>
+      <c r="J17" s="329"/>
+      <c r="K17" s="329"/>
+      <c r="L17" s="329"/>
+      <c r="M17" s="329"/>
+      <c r="N17" s="329"/>
+      <c r="O17" s="329"/>
+      <c r="P17" s="329"/>
+      <c r="Q17" s="329"/>
+      <c r="R17" s="329"/>
+      <c r="S17" s="329"/>
+      <c r="T17" s="329"/>
+      <c r="U17" s="329"/>
+      <c r="V17" s="329"/>
+      <c r="W17" s="329"/>
+      <c r="X17" s="329"/>
+      <c r="Y17" s="329"/>
+      <c r="Z17" s="329"/>
+      <c r="AA17" s="330"/>
     </row>
     <row r="18" spans="1:27" ht="16" thickTop="1">
       <c r="A18" s="11"/>
@@ -25804,11 +25833,11 @@
       </c>
       <c r="D22" s="132" t="str">
         <f>IF(COUNTIF(Skips,CostRemaining[[#This Row],[Cost]])&gt;0,"IGNORE",CostRemaining[Kind]&amp;"-"&amp;CostRemaining[Resource])</f>
-        <v>IGNORE</v>
+        <v>Building-Elixir</v>
       </c>
       <c r="E22" s="54">
         <f ca="1">IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;MATCH(TRUE,INDEX(CostRemaining[[#This Row],[1]:[12]]&lt;&gt;0,),0),Upgrades[#Headers],0),FALSE),"")</f>
-        <v>700000</v>
+        <v>1500000</v>
       </c>
       <c r="F22" s="55">
         <f ca="1">IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F26,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G26:G26)),0)</f>
@@ -25840,7 +25869,7 @@
       </c>
       <c r="M22" s="55">
         <f ca="1">IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F26,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G26:N26)),0)</f>
-        <v>700000</v>
+        <v>0</v>
       </c>
       <c r="N22" s="55">
         <f ca="1">IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F26,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G26:O26)),0)</f>
@@ -25859,8 +25888,8 @@
         <v>0</v>
       </c>
       <c r="R22" s="55">
-        <f>IF(CostRemaining[[#This Row],[MatchStr]]="IGNORE",0,SUM(CostRemaining[[#This Row],[1]:[12]]))</f>
-        <v>0</v>
+        <f ca="1">IF(CostRemaining[[#This Row],[MatchStr]]="IGNORE",0,SUM(CostRemaining[[#This Row],[1]:[12]]))</f>
+        <v>4500000</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -26781,7 +26810,7 @@
       </c>
       <c r="K35" s="55">
         <f ca="1">IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F39,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G39:L39)),0)</f>
-        <v>8925000</v>
+        <v>6750000</v>
       </c>
       <c r="L35" s="55">
         <f ca="1">IF(VALUE(CostRemaining[#Headers])&lt;='Construction Dashboard'!$F39,IFERROR(VLOOKUP(CostRemaining[[#This Row],[Cost]],Upgrades[],MATCH("C"&amp;CostRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G39:M39)),0)</f>
@@ -26809,7 +26838,7 @@
       </c>
       <c r="R35" s="55">
         <f ca="1">IF(CostRemaining[[#This Row],[MatchStr]]="IGNORE",0,SUM(CostRemaining[[#This Row],[1]:[12]]))</f>
-        <v>43725000</v>
+        <v>41550000</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -29223,35 +29252,35 @@
     </row>
     <row r="70" spans="1:27" ht="16" thickBot="1"/>
     <row r="71" spans="1:27" ht="32" thickTop="1" thickBot="1">
-      <c r="A71" s="325" t="s">
+      <c r="A71" s="328" t="s">
         <v>211</v>
       </c>
-      <c r="B71" s="326"/>
-      <c r="C71" s="326"/>
-      <c r="D71" s="326"/>
-      <c r="E71" s="326"/>
-      <c r="F71" s="326"/>
-      <c r="G71" s="326"/>
-      <c r="H71" s="326"/>
-      <c r="I71" s="326"/>
-      <c r="J71" s="326"/>
-      <c r="K71" s="326"/>
-      <c r="L71" s="326"/>
-      <c r="M71" s="326"/>
-      <c r="N71" s="326"/>
-      <c r="O71" s="326"/>
-      <c r="P71" s="326"/>
-      <c r="Q71" s="326"/>
-      <c r="R71" s="326"/>
-      <c r="S71" s="326"/>
-      <c r="T71" s="326"/>
-      <c r="U71" s="326"/>
-      <c r="V71" s="326"/>
-      <c r="W71" s="326"/>
-      <c r="X71" s="326"/>
-      <c r="Y71" s="326"/>
-      <c r="Z71" s="326"/>
-      <c r="AA71" s="327"/>
+      <c r="B71" s="329"/>
+      <c r="C71" s="329"/>
+      <c r="D71" s="329"/>
+      <c r="E71" s="329"/>
+      <c r="F71" s="329"/>
+      <c r="G71" s="329"/>
+      <c r="H71" s="329"/>
+      <c r="I71" s="329"/>
+      <c r="J71" s="329"/>
+      <c r="K71" s="329"/>
+      <c r="L71" s="329"/>
+      <c r="M71" s="329"/>
+      <c r="N71" s="329"/>
+      <c r="O71" s="329"/>
+      <c r="P71" s="329"/>
+      <c r="Q71" s="329"/>
+      <c r="R71" s="329"/>
+      <c r="S71" s="329"/>
+      <c r="T71" s="329"/>
+      <c r="U71" s="329"/>
+      <c r="V71" s="329"/>
+      <c r="W71" s="329"/>
+      <c r="X71" s="329"/>
+      <c r="Y71" s="329"/>
+      <c r="Z71" s="329"/>
+      <c r="AA71" s="330"/>
     </row>
     <row r="72" spans="1:27" ht="16" thickTop="1">
       <c r="A72" s="11"/>
@@ -29489,11 +29518,11 @@
       </c>
       <c r="D76" s="132" t="str">
         <f>IF(COUNTIF(Skips,TimeRemaining[[#This Row],[Time]])&gt;0,"IGNORE",TimeRemaining[Kind]&amp;"-"&amp;TimeRemaining[Resource])</f>
-        <v>IGNORE</v>
+        <v>Building-Elixir</v>
       </c>
       <c r="E76" s="62">
         <f ca="1">IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;MATCH(TRUE,INDEX(TimeRemaining[[#This Row],[1]:[12]]&lt;&gt;0,),0),Upgrades[#Headers],0),FALSE),"")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F76" s="61">
         <f ca="1">IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F26,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G26:G26)),0)</f>
@@ -29525,7 +29554,7 @@
       </c>
       <c r="M76" s="61">
         <f ca="1">IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F26,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G26:N26)),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N76" s="61">
         <f ca="1">IF(VALUE(TimeRemaining[#Headers])&lt;='Construction Dashboard'!$F26,IFERROR(VLOOKUP(TimeRemaining[[#This Row],[Time]],Upgrades[],MATCH("T"&amp;TimeRemaining[#Headers],Upgrades[#Headers],0),FALSE),0)*MAX(0,SUM('Construction Dashboard'!$G26:O26)),0)</f>
@@ -29544,8 +29573,8 @@
         <v>0</v>
       </c>
       <c r="R76" s="61">
-        <f>IF(TimeRemaining[[#This Row],[MatchStr]]="IGNORE",0,SUM(TimeRemaining[[#This Row],[1]:[12]]))</f>
-        <v>0</v>
+        <f ca="1">IF(TimeRemaining[[#This Row],[MatchStr]]="IGNORE",0,SUM(TimeRemaining[[#This Row],[1]:[12]]))</f>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:27">
@@ -32914,7 +32943,7 @@
     <mergeCell ref="A1:AA1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsErrors" dxfId="47" priority="3">
+    <cfRule type="containsErrors" dxfId="49" priority="3">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>